<commit_message>
rf & knn models with 2 attributes
also modified training and testing  with the correct data
</commit_message>
<xml_diff>
--- a/info/model_results_comparative_table.xlsx
+++ b/info/model_results_comparative_table.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kiko Sánchez\Desktop\Ubiqum\Course 2\Task 3\multiple_regression\blackwells_multiple_regression\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{607FD7F3-8148-42EF-9001-AE42BC622BBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580ED6C7-1B49-49F2-AD02-8871D65302FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>RF</t>
   </si>
@@ -72,12 +72,27 @@
   </si>
   <si>
     <t>rmse:315.14, Rsq:0.82, mae:181.16</t>
+  </si>
+  <si>
+    <t>2 att</t>
+  </si>
+  <si>
+    <t>(mtry:2) rmse:153.41, Rsq:0.94, mae:84.96</t>
+  </si>
+  <si>
+    <t>rmse:249.41, Rsq:0.87, mae:148.6</t>
+  </si>
+  <si>
+    <t>(k:5) rmse:241.47, Rsq:0.85, mae:115.35</t>
+  </si>
+  <si>
+    <t>rmse:312.05, Rsq:0.82, mae:179.98</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -102,10 +117,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -114,12 +138,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,84 +467,104 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.26953125" customWidth="1"/>
-    <col min="2" max="2" width="29.81640625" customWidth="1"/>
-    <col min="3" max="3" width="29.08984375" customWidth="1"/>
-    <col min="4" max="4" width="28.7265625" customWidth="1"/>
-    <col min="5" max="5" width="27.90625" customWidth="1"/>
+    <col min="2" max="3" width="31.7265625" customWidth="1"/>
+    <col min="4" max="4" width="34" customWidth="1"/>
+    <col min="5" max="6" width="28.7265625" customWidth="1"/>
+    <col min="7" max="7" width="28.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>2</v>
       </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>